<commit_message>
syntax correction in rules tables + additional comments
</commit_message>
<xml_diff>
--- a/docs/sbr_decision_tables.xlsx
+++ b/docs/sbr_decision_tables.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="102">
   <si>
     <t>Required Skills</t>
   </si>
@@ -255,6 +255,9 @@
     <t>"Herbert"</t>
   </si>
   <si>
+    <t>TAR_EZ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i/>
@@ -270,7 +273,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>"KULANZ","EXKASSO_L"</t>
+      <t>["GOÄ","AMNOG"]</t>
     </r>
     <r>
       <rPr>
@@ -283,7 +286,13 @@
     </r>
   </si>
   <si>
-    <t>TAR_EZ</t>
+    <t>"Andreas"</t>
+  </si>
+  <si>
+    <t>[ ]</t>
+  </si>
+  <si>
+    <t>"Emma"</t>
   </si>
   <si>
     <r>
@@ -301,7 +310,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>["GOÄ","AMNOG"]</t>
+      <t>["GOÄ","AMNOG","TAR_AB"]</t>
     </r>
     <r>
       <rPr>
@@ -314,10 +323,10 @@
     </r>
   </si>
   <si>
-    <t>"Andreas"</t>
-  </si>
-  <si>
-    <t>[ ]</t>
+    <t>Für "Kleinvieh" wird sie dabei zusätzlich unterstützt von Sonja</t>
+  </si>
+  <si>
+    <t>"Sonja"</t>
   </si>
   <si>
     <r>
@@ -335,7 +344,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>"EXKASSO_S","EXKASSO_M"</t>
+      <t>["GOZ","TAR_EZ"]</t>
     </r>
     <r>
       <rPr>
@@ -348,7 +357,7 @@
     </r>
   </si>
   <si>
-    <t>"Emma"</t>
+    <t>"Xaver"</t>
   </si>
   <si>
     <r>
@@ -366,7 +375,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>"EXKASSO_S"</t>
+      <t>["HeilM-RL"]</t>
     </r>
     <r>
       <rPr>
@@ -379,6 +388,12 @@
     </r>
   </si>
   <si>
+    <t>"Hanna"</t>
+  </si>
+  <si>
+    <t>"Bernd"</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i/>
@@ -394,7 +409,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>["GOÄ","AMNOG","TAR_AB"]</t>
+      <t>["TAR_AB","TAR_EZ"]</t>
     </r>
     <r>
       <rPr>
@@ -407,10 +422,13 @@
     </r>
   </si>
   <si>
-    <t>Für "Kleinvieh" wird sie dabei zusätzlich unterstützt von Sonja</t>
-  </si>
-  <si>
-    <t>"Sonja"</t>
+    <t>"Tom"</t>
+  </si>
+  <si>
+    <t>Tom kennt das gesamte Tarifwerk und unterstützt Emma bei der Rechnungsfreigabe im mittleren Bereich</t>
+  </si>
+  <si>
+    <t>TAR_ES</t>
   </si>
   <si>
     <r>
@@ -428,7 +446,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>["GOZ","TAR_EZ"]</t>
+      <t>["SH","TAR_ES"]</t>
     </r>
     <r>
       <rPr>
@@ -441,7 +459,52 @@
     </r>
   </si>
   <si>
-    <t>"Xaver"</t>
+    <t>Emma macht auch GOÄ, regiliert aber nicht, gibt dafür aber bis zu mittleren Beträgen frei.</t>
+  </si>
+  <si>
+    <t>Andreas macht GOÄ/Arzneimittel, reguliert nach allg. Basistarifen hat aber keine weiteren Rechte.</t>
+  </si>
+  <si>
+    <t>Herbert ist auch derjenige, der auf Kulanz regulieren darf und große Beträge freigeben muss.</t>
+  </si>
+  <si>
+    <t>Wenn es jedoch um Heilmittel geht, wird Herbert noch dazu gezogen.</t>
+  </si>
+  <si>
+    <t>Ines macht grundsätzlich alles, was intern vertraulich gehandhabt werden muss.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xaver macht GOZ und reguliert nach Zusatztarifen </t>
+  </si>
+  <si>
+    <t>Hanna war mal Heilpraktikerin. Weder reguliert sie noch hat sie Rechte zur Freigabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bernd ist gelernter Optiker, reguliert entsprechende Tarife (und darf auch Kulanzregelungen treffen) </t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Ist der Leistungsempfänger ein Mitarbeiter, so muss dies intern vertraulich behandelt werden</t>
+  </si>
+  <si>
+    <t>Wenn es nicht um die Standard-Rechnungen geht, muss jemand rann, der ggf. auch Kulanzregelungen treffen kann</t>
+  </si>
+  <si>
+    <t>Auch für wichtige Kunden sind ggf. Kulanzen bei der Berechnung des Erstattungsbetrags gefragt</t>
+  </si>
+  <si>
+    <t>Für VIPs werden ferner Erstattungsbeträge bis 500,-- als klein betrachtet ("Durchwinken")</t>
+  </si>
+  <si>
+    <t>Ansonsten werden für unterschiedliche Freigabehöhen entsprechende Rechte benötigt...</t>
+  </si>
+  <si>
+    <t>Unabhängig vom Kundenstatus wird alles über 500,-- als "Large" angesehen</t>
+  </si>
+  <si>
+    <t>... und zwar in den Stufen "Small" / "Medium" / "Large"</t>
   </si>
   <si>
     <r>
@@ -459,7 +522,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>["HeilM-RL"]</t>
+      <t>["KULANZ","EXKASSO_L"]</t>
     </r>
     <r>
       <rPr>
@@ -472,12 +535,6 @@
     </r>
   </si>
   <si>
-    <t>"Hanna"</t>
-  </si>
-  <si>
-    <t>"Bernd"</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <i/>
@@ -493,7 +550,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>"KULANZ"</t>
+      <t>["EXKASSO_S","EXKASSO_M"]</t>
     </r>
     <r>
       <rPr>
@@ -521,7 +578,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>["TAR_AB","TAR_EZ"]</t>
+      <t>["EXKASSO_S"]</t>
     </r>
     <r>
       <rPr>
@@ -549,7 +606,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>"EXKASSO_M"</t>
+      <t>["EXKASSO_M"]</t>
     </r>
     <r>
       <rPr>
@@ -562,15 +619,6 @@
     </r>
   </si>
   <si>
-    <t>"Tom"</t>
-  </si>
-  <si>
-    <t>Tom kennt das gesamte Tarifwerk und unterstützt Emma bei der Rechnungsfreigabe im mittleren Bereich</t>
-  </si>
-  <si>
-    <t>TAR_ES</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <i/>
@@ -586,7 +634,7 @@
         <color theme="1"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>["SH","TAR_ES"]</t>
+      <t>["KULANZ"]</t>
     </r>
     <r>
       <rPr>
@@ -599,38 +647,141 @@
     </r>
   </si>
   <si>
-    <t>Emma macht auch GOÄ, regiliert aber nicht, gibt dafür aber bis zu mittleren Beträgen frei.</t>
-  </si>
-  <si>
-    <t>Andreas macht GOÄ/Arzneimittel, reguliert nach allg. Basistarifen hat aber keine weiteren Rechte.</t>
-  </si>
-  <si>
-    <t>Herbert ist auch derjenige, der auf Kulanz regulieren darf und große Beträge freigeben muss.</t>
-  </si>
-  <si>
-    <t>Wenn es jedoch um Heilmittel geht, wird Herbert noch dazu gezogen.</t>
-  </si>
-  <si>
-    <t>Ines macht grundsätzlich alles, was intern vertraulich gehandhabt werden muss.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xaver macht GOZ und reguliert nach Zusatztarifen </t>
-  </si>
-  <si>
-    <t>Hanna war mal Heilpraktikerin. Weder reguliert sie noch hat sie Rechte zur Freigabe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bernd ist gelernter Optiker, reguliert entsprechende Tarife (und darf auch Kulanzregelungen treffen) </t>
-  </si>
-  <si>
-    <t>RI</t>
+    <t>Für die gebührenrechliche Prüfung sind Kenntniss der entspr. Gebührenordnungen und Verordnungen erforderlich:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>ebühren</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">rdnung der </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Ä</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>rzte</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>ebühren</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">rdnung der </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>ahnärzte</t>
+    </r>
+  </si>
+  <si>
+    <t>Sehhilfen</t>
+  </si>
+  <si>
+    <t>Gesetz zur Neuordnung des Arzneimittelmarktes</t>
+  </si>
+  <si>
+    <t>Heilmittel-Richtlinie</t>
+  </si>
+  <si>
+    <t>Für die Berechnung der Erstattungbeträge ist Kenntnis zu den produktspezifischen Tarifen erforderlich</t>
+  </si>
+  <si>
+    <t>Tarifgruppe "Allgemeine Basistarife"</t>
+  </si>
+  <si>
+    <t>Tarifgruppe "Ergänzungs- und Zusatztarife"</t>
+  </si>
+  <si>
+    <t>Tarifgruppe "Ergänzungstarife für Sehhilfen"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -687,6 +838,23 @@
       <color theme="1" tint="0.499984740745262"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -946,7 +1114,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1072,8 +1240,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1114,15 +1314,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1137,6 +1328,48 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1144,62 +1377,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="157">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1262,6 +1465,22 @@
     <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1324,6 +1543,22 @@
     <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1653,7 +1888,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1668,17 +1903,18 @@
     <col min="5" max="5" width="36.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="36.5" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="36.5" style="2" customWidth="1"/>
-    <col min="8" max="12" width="25.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="3" style="2" customWidth="1"/>
+    <col min="9" max="12" width="25.6640625" style="2" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" ht="23" customHeight="1">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" ht="23" customHeight="1" thickBot="1">
+      <c r="B1" s="34"/>
+    </row>
+    <row r="2" spans="1:9" ht="23" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1701,11 +1937,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="23" customHeight="1" thickTop="1">
+    <row r="3" spans="1:9" ht="23" customHeight="1" thickTop="1">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -1717,16 +1953,19 @@
       <c r="E3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="23" customHeight="1">
+      <c r="I3" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23" customHeight="1">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="9" t="s">
         <v>33</v>
       </c>
@@ -1736,16 +1975,19 @@
       <c r="E4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="21" t="s">
+      <c r="F4" s="20"/>
+      <c r="G4" s="18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="23" customHeight="1">
+      <c r="I4" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="23" customHeight="1">
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="9" t="s">
         <v>36</v>
       </c>
@@ -1755,16 +1997,19 @@
       <c r="E5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="20"/>
+      <c r="G5" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="23" customHeight="1">
+      <c r="I5" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="23" customHeight="1">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="9" t="s">
         <v>37</v>
       </c>
@@ -1774,16 +2019,19 @@
       <c r="E6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="21" t="s">
+      <c r="F6" s="20"/>
+      <c r="G6" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="23" customHeight="1">
+      <c r="I6" s="32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23" customHeight="1">
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="9" t="s">
         <v>39</v>
       </c>
@@ -1793,16 +2041,19 @@
       <c r="E7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="21" t="s">
+      <c r="F7" s="20"/>
+      <c r="G7" s="18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="23" customHeight="1">
+      <c r="I7" s="42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="23" customHeight="1">
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="9" t="s">
         <v>41</v>
       </c>
@@ -1812,16 +2063,19 @@
       <c r="E8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="20"/>
+      <c r="G8" s="18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="23" customHeight="1">
+      <c r="I8" s="32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23" customHeight="1">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="9" t="s">
         <v>43</v>
       </c>
@@ -1831,16 +2085,16 @@
       <c r="E9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="21" t="s">
+      <c r="F9" s="20"/>
+      <c r="G9" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="23" customHeight="1">
+    <row r="10" spans="1:9" ht="23" customHeight="1">
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="39" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -1852,50 +2106,59 @@
       <c r="E10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="21" t="s">
+      <c r="F10" s="20"/>
+      <c r="G10" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="23" customHeight="1">
+      <c r="I10" s="32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="23" customHeight="1">
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="29" t="s">
+      <c r="B11" s="36"/>
+      <c r="C11" s="38" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="20"/>
+      <c r="G11" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="23" customHeight="1">
+      <c r="I11" s="32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="23" customHeight="1">
       <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="23" customHeight="1">
+      <c r="E12" s="37"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="23" customHeight="1">
       <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="13" t="s">
         <v>16</v>
       </c>
@@ -1905,16 +2168,16 @@
       <c r="E13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="23" customHeight="1">
+      <c r="F13" s="20"/>
+      <c r="G13" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="23" customHeight="1">
       <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="13" t="s">
         <v>16</v>
       </c>
@@ -1924,9 +2187,12 @@
       <c r="E14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="21" t="s">
-        <v>74</v>
+      <c r="F14" s="20"/>
+      <c r="G14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1950,7 +2216,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1959,20 +2225,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="39.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="39.6640625" style="2" customWidth="1"/>
-    <col min="8" max="12" width="25.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="33" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="33" style="2" customWidth="1"/>
+    <col min="8" max="8" width="3" style="2" customWidth="1"/>
+    <col min="9" max="12" width="25.6640625" style="2" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" ht="23" customHeight="1">
+      <c r="A1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" ht="23" customHeight="1" thickBot="1">
+      <c r="B1" s="34"/>
+    </row>
+    <row r="2" spans="1:9" ht="23" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1988,18 +2256,18 @@
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="23" customHeight="1" thickTop="1">
+    <row r="3" spans="1:9" ht="23" customHeight="1" thickTop="1">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="21" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -2011,14 +2279,17 @@
       <c r="E3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="23" customHeight="1">
+      <c r="I3" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23" customHeight="1">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -2034,14 +2305,17 @@
       <c r="E4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="21" t="s">
+      <c r="F4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="23" customHeight="1">
+      <c r="I4" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="23" customHeight="1">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -2057,21 +2331,24 @@
       <c r="E5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="23" customHeight="1">
+      <c r="I5" s="32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="23" customHeight="1">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="38" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -2080,66 +2357,78 @@
       <c r="E6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="23" customHeight="1">
+      <c r="I6" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23" customHeight="1">
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="14" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="39" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="23" customHeight="1">
+      <c r="I7" s="32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="23" customHeight="1">
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="26"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="23" customHeight="1">
+      <c r="I8" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23" customHeight="1">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="16"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="18" t="s">
         <v>31</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2168,11 +2457,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="41.1640625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" style="32" customWidth="1"/>
-    <col min="4" max="5" width="29.5" style="32" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" style="23" customWidth="1"/>
+    <col min="4" max="5" width="29.5" style="23" customWidth="1"/>
     <col min="6" max="6" width="1.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="40" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="31" customWidth="1"/>
     <col min="8" max="9" width="25.6640625" style="2" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -2181,22 +2470,22 @@
       <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="23" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2204,180 +2493,180 @@
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="G3" s="41" t="s">
-        <v>80</v>
+      <c r="E3" s="28"/>
+      <c r="G3" s="32" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="23" customHeight="1">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="G4" s="41" t="s">
-        <v>79</v>
+      <c r="E4" s="30"/>
+      <c r="G4" s="32" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="23" customHeight="1">
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="39" t="s">
+      <c r="B5" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="G5" s="41" t="s">
-        <v>78</v>
+      <c r="E5" s="30"/>
+      <c r="G5" s="32" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="23" customHeight="1">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="39" t="s">
+      <c r="B6" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="G6" s="41" t="s">
-        <v>77</v>
+      <c r="D6" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="G6" s="32" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="23" customHeight="1">
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="39"/>
-      <c r="G7" s="41" t="s">
-        <v>76</v>
+      <c r="B7" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="G7" s="32" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="23" customHeight="1">
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="38" t="s">
+      <c r="B8" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="39"/>
-      <c r="G8" s="41" t="s">
-        <v>62</v>
+      <c r="E8" s="30"/>
+      <c r="G8" s="32" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="23" customHeight="1">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="39"/>
-      <c r="G9" s="41" t="s">
-        <v>81</v>
+      <c r="B9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="G9" s="32" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="23" customHeight="1">
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="39"/>
-      <c r="G10" s="41" t="s">
-        <v>82</v>
+      <c r="B10" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="G10" s="32" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="23" customHeight="1">
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="39"/>
-      <c r="G11" s="41" t="s">
-        <v>83</v>
+      <c r="B11" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="G11" s="32" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="23" customHeight="1">
       <c r="A12" s="8">
         <v>9</v>
       </c>
-      <c r="B12" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="39"/>
-      <c r="G12" s="41" t="s">
-        <v>73</v>
+      <c r="B12" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="G12" s="32" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync: New rules for Leistungsabrechnung, not working
</commit_message>
<xml_diff>
--- a/docs/sbr_decision_tables.xlsx
+++ b/docs/sbr_decision_tables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="-19340" windowWidth="32560" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="1155" yWindow="-19335" windowWidth="29040" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fähigkeiten" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,6 @@
     <t>AMNOG</t>
   </si>
   <si>
-    <t>"Phisiotherapie"</t>
-  </si>
-  <si>
     <t>HeilM-RL</t>
   </si>
   <si>
@@ -775,6 +772,9 @@
   </si>
   <si>
     <t>Tarifgruppe "Ergänzungstarife für Sehhilfen"</t>
+  </si>
+  <si>
+    <t>"Physiotherapie"</t>
   </si>
 </sst>
 </file>
@@ -1371,6 +1371,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1398,171 +1401,173 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="157">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1891,30 +1896,30 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="2" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="36.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="36.5" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="36.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="3" style="2" customWidth="1"/>
-    <col min="9" max="12" width="25.6640625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="12" width="25.625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23" customHeight="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-    </row>
-    <row r="2" spans="1:9" ht="23" customHeight="1" thickBot="1">
+      <c r="B1" s="35"/>
+    </row>
+    <row r="2" spans="1:9" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1937,11 +1942,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="23" customHeight="1" thickTop="1">
+    <row r="3" spans="1:9" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -1958,14 +1963,14 @@
         <v>32</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="23" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="9" t="s">
         <v>33</v>
       </c>
@@ -1980,14 +1985,14 @@
         <v>34</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="23" customHeight="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="9" t="s">
         <v>36</v>
       </c>
@@ -2002,14 +2007,14 @@
         <v>32</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="23" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="9" t="s">
         <v>37</v>
       </c>
@@ -2024,14 +2029,14 @@
         <v>38</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="23" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="9" t="s">
         <v>39</v>
       </c>
@@ -2045,17 +2050,17 @@
       <c r="G7" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="23" customHeight="1">
+      <c r="I7" s="33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="9" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>16</v>
@@ -2065,19 +2070,19 @@
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="23" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>16</v>
@@ -2087,14 +2092,14 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="23" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="40" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -2104,61 +2109,61 @@
         <v>16</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="23" customHeight="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="38" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="39" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="38" t="s">
-        <v>47</v>
+      <c r="E11" s="39" t="s">
+        <v>46</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="23" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="20"/>
       <c r="G12" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="23" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="13" t="s">
         <v>16</v>
       </c>
@@ -2166,18 +2171,18 @@
         <v>16</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="23" customHeight="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="13" t="s">
         <v>16</v>
       </c>
@@ -2185,14 +2190,14 @@
         <v>16</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2222,25 +2227,25 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.625" style="2" customWidth="1"/>
     <col min="3" max="4" width="33" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="33" style="2" customWidth="1"/>
     <col min="8" max="8" width="3" style="2" customWidth="1"/>
-    <col min="9" max="12" width="25.6640625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="12" width="25.625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23" customHeight="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="34"/>
-    </row>
-    <row r="2" spans="1:9" ht="23" customHeight="1" thickBot="1">
+      <c r="B1" s="35"/>
+    </row>
+    <row r="2" spans="1:9" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -2263,7 +2268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="23" customHeight="1" thickTop="1">
+    <row r="3" spans="1:9" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2286,10 +2291,10 @@
         <v>17</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="23" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -2297,7 +2302,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>16</v>
@@ -2312,10 +2317,10 @@
         <v>22</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="23" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -2338,17 +2343,17 @@
         <v>22</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="23" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="39" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -2364,16 +2369,16 @@
         <v>26</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="23" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="39" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="40" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="13" t="s">
@@ -2386,16 +2391,16 @@
         <v>26</v>
       </c>
       <c r="I7" s="32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="23" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="13" t="s">
         <v>16</v>
       </c>
@@ -2406,15 +2411,15 @@
         <v>29</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="23" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="37"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="13" t="s">
         <v>16</v>
       </c>
@@ -2428,7 +2433,7 @@
         <v>31</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2454,27 +2459,27 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="41.1640625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="41.125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="48.625" style="23" customWidth="1"/>
     <col min="4" max="5" width="29.5" style="23" customWidth="1"/>
-    <col min="6" max="6" width="1.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="31" customWidth="1"/>
-    <col min="8" max="9" width="25.6640625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="1.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.625" style="31" customWidth="1"/>
+    <col min="8" max="9" width="25.625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23" customHeight="1">
+    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="22"/>
     </row>
-    <row r="2" spans="1:7" ht="23" customHeight="1" thickBot="1">
+    <row r="2" spans="1:7" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>12</v>
@@ -2489,7 +2494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="23" customHeight="1" thickTop="1">
+    <row r="3" spans="1:7" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2497,35 +2502,35 @@
         <v>16</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="28"/>
       <c r="G3" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="23" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>51</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>52</v>
       </c>
       <c r="E4" s="30"/>
       <c r="G4" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="23" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -2533,53 +2538,53 @@
         <v>16</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="30"/>
       <c r="G5" s="32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="23" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="30"/>
       <c r="G6" s="32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="23" customHeight="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="30"/>
       <c r="G7" s="32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="23" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -2587,86 +2592,86 @@
         <v>16</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="30"/>
       <c r="G8" s="32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="23" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
       <c r="B9" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="30" t="s">
         <v>61</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>62</v>
       </c>
       <c r="E9" s="30"/>
       <c r="G9" s="32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="23" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>63</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>64</v>
       </c>
       <c r="E10" s="30"/>
       <c r="G10" s="32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="23" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="30"/>
       <c r="G11" s="32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="23" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>9</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="30" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>67</v>
       </c>
       <c r="E12" s="30"/>
       <c r="G12" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>